<commit_message>
diccionario de datos y metodos add
</commit_message>
<xml_diff>
--- a/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
+++ b/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablofernandezsato/Desktop/BBDD - LIBRO/Bibliov2-1/DIAGRAMAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablofernandezsato/Desktop/Git/Libreriav2/DIAGRAMAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5DB0F5-6A78-DC4D-85E9-A87F7B34D7CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FEDE44-2DBC-7043-AEC4-DA7628FFD65B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7040" yWindow="500" windowWidth="25440" windowHeight="14040" xr2:uid="{E2514F55-DB76-7447-8476-23FD56A879E1}"/>
+    <workbookView xWindow="-35640" yWindow="1260" windowWidth="25440" windowHeight="14040" xr2:uid="{E2514F55-DB76-7447-8476-23FD56A879E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="66">
   <si>
     <t>LIBRO</t>
   </si>
@@ -111,9 +111,6 @@
     <t>UBICACIÓN DONDE ESTÁ</t>
   </si>
   <si>
-    <t>LIBRO_AUTOR</t>
-  </si>
-  <si>
     <t>AUTOR</t>
   </si>
   <si>
@@ -222,23 +219,26 @@
     <t>DIBUJANTE</t>
   </si>
   <si>
-    <t>DIBUJANTE SI O NO</t>
-  </si>
-  <si>
     <t>LIBRO_BALDA</t>
   </si>
   <si>
     <t>ESCRITOR</t>
   </si>
   <si>
-    <t>ESCRITOR SI O NO</t>
+    <t>LIBRO_ESCRITOR</t>
+  </si>
+  <si>
+    <t>LIBRO_ESCRITOR_DIBUJANTE</t>
+  </si>
+  <si>
+    <t>ALIAS DEL DIBUJANTE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +328,14 @@
       <color rgb="FFFF0000"/>
       <name val="Calibri (Cuerpo)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -373,7 +381,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -823,11 +831,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -995,6 +1044,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1013,29 +1086,59 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1351,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896DC84-666B-2C40-BFB0-FA171D076670}">
-  <dimension ref="B5:H80"/>
+  <dimension ref="B5:H94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1365,15 +1468,15 @@
   <sheetData>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:8" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="63" t="s">
+      <c r="B6" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
     </row>
     <row r="7" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
@@ -1400,7 +1503,7 @@
     </row>
     <row r="8" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B8" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>20</v>
@@ -1409,7 +1512,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>17</v>
@@ -1522,7 +1625,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>18</v>
@@ -1545,7 +1648,7 @@
         <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>18</v>
@@ -1559,7 +1662,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>15</v>
@@ -1568,7 +1671,7 @@
         <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>18</v>
@@ -1605,53 +1708,53 @@
     </row>
     <row r="17" spans="2:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B17" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="66">
+      <c r="D17" s="59">
         <v>3</v>
       </c>
-      <c r="E17" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="67" t="s">
+      <c r="E17" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="66">
+      <c r="D18" s="59">
         <v>2</v>
       </c>
-      <c r="E18" s="66" t="s">
-        <v>58</v>
-      </c>
-      <c r="F18" s="66" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="66" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="67" t="s">
+      <c r="E18" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="59" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="60" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="52" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>20</v>
@@ -1660,52 +1763,52 @@
         <v>3</v>
       </c>
       <c r="E19" s="54" t="s">
+        <v>58</v>
+      </c>
+      <c r="F19" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="55" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="57" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="62">
+        <v>3</v>
+      </c>
+      <c r="E20" s="62" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="55" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="68" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="69">
-        <v>3</v>
-      </c>
-      <c r="E20" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="69" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="69" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="70" t="s">
+      <c r="F20" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="62" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="63" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
-      <c r="H22" s="63"/>
+      <c r="B22" s="64" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
     </row>
     <row r="23" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
@@ -1732,7 +1835,7 @@
     </row>
     <row r="24" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>20</v>
@@ -1741,7 +1844,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -1778,7 +1881,7 @@
     </row>
     <row r="26" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>15</v>
@@ -1787,10 +1890,10 @@
         <v>50</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>17</v>
@@ -1801,15 +1904,15 @@
     </row>
     <row r="27" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="63" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
-      <c r="H28" s="63"/>
+      <c r="B28" s="64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="64"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="64"/>
+      <c r="F28" s="64"/>
+      <c r="G28" s="64"/>
+      <c r="H28" s="64"/>
     </row>
     <row r="29" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
@@ -1836,7 +1939,7 @@
     </row>
     <row r="30" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B30" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
         <v>15</v>
@@ -1845,7 +1948,7 @@
         <v>50</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>18</v>
@@ -1859,7 +1962,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>15</v>
@@ -1868,7 +1971,7 @@
         <v>100</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>18</v>
@@ -1882,7 +1985,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>15</v>
@@ -1891,686 +1994,670 @@
         <v>50</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="64" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+    </row>
+    <row r="37" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="12" t="s">
+      <c r="C38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" s="2">
+        <v>50</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="4">
+        <v>100</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="4">
+        <v>50</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="C33" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4" t="s">
+      <c r="C44" s="71"/>
+      <c r="D44" s="71"/>
+      <c r="E44" s="71"/>
+      <c r="F44" s="71"/>
+      <c r="G44" s="71"/>
+      <c r="H44" s="71"/>
+    </row>
+    <row r="45" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="72" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="72" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" s="72" t="s">
+        <v>4</v>
+      </c>
+      <c r="F45" s="72" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="73" t="s">
+        <v>52</v>
+      </c>
+      <c r="C46" s="74" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="75">
+        <v>5</v>
+      </c>
+      <c r="E46" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="F46" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="G46" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="C47" s="78" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" s="79">
+        <v>100</v>
+      </c>
+      <c r="E47" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H47" s="80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="81" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" s="82" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" s="83">
+        <v>50</v>
+      </c>
+      <c r="E48" s="83" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="83" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="83" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="84" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="86" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" s="87">
+        <v>50</v>
+      </c>
+      <c r="E49" s="87" t="s">
         <v>65</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B34" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6" t="s">
+      <c r="F49" s="87" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="88" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="51" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B52" s="68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" s="69"/>
+      <c r="D52" s="69"/>
+      <c r="E52" s="69"/>
+      <c r="F52" s="69"/>
+      <c r="G52" s="69"/>
+      <c r="H52" s="70"/>
+    </row>
+    <row r="53" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H53" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" s="38">
+        <v>50</v>
+      </c>
+      <c r="E54" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="63" t="s">
+      <c r="F54" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H54" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="65" t="s">
+        <v>37</v>
+      </c>
+      <c r="C56" s="66"/>
+      <c r="D56" s="66"/>
+      <c r="E56" s="66"/>
+      <c r="F56" s="66"/>
+      <c r="G56" s="66"/>
+      <c r="H56" s="67"/>
+    </row>
+    <row r="57" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E57" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G57" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-    </row>
-    <row r="39" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
+      <c r="C58" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" s="28">
+        <v>50</v>
+      </c>
+      <c r="E58" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F58" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G58" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H58" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B59" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C59" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="31">
+        <v>100</v>
+      </c>
+      <c r="E59" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" s="34">
+        <v>3</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="41"/>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
+      <c r="F61" s="40"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="40"/>
+    </row>
+    <row r="62" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="64" t="s">
+        <v>40</v>
+      </c>
+      <c r="C63" s="64"/>
+      <c r="D63" s="64"/>
+      <c r="E63" s="64"/>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="64"/>
+    </row>
+    <row r="64" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="17" t="s">
+      <c r="C64" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D64" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E64" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F64" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G64" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H64" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="37" t="s">
+    <row r="65" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="38">
+      <c r="D65" s="2">
         <v>50</v>
       </c>
-      <c r="E40" s="38" t="s">
+      <c r="E65" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F40" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="57" t="s">
+      <c r="F65" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" s="6">
+        <v>50</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H66" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="51"/>
+      <c r="C67" s="50"/>
+      <c r="D67" s="50"/>
+      <c r="E67" s="50"/>
+      <c r="F67" s="50"/>
+      <c r="G67" s="50"/>
+      <c r="H67" s="50"/>
+    </row>
+    <row r="68" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B68" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="C68" s="66"/>
+      <c r="D68" s="66"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
+      <c r="G68" s="66"/>
+      <c r="H68" s="67"/>
+    </row>
+    <row r="69" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D69" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E69" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F69" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G69" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H69" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C70" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" s="28">
+        <v>50</v>
+      </c>
+      <c r="E70" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F70" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B71" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" s="31">
+        <v>100</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="58"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="59"/>
-    </row>
-    <row r="43" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D43" s="26" t="s">
+      <c r="C72" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="34">
         <v>3</v>
       </c>
-      <c r="E43" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G43" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="44" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D44" s="28">
-        <v>50</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="F44" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H44" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C45" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="31">
-        <v>100</v>
-      </c>
-      <c r="E45" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H45" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="46" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="33" t="s">
+      <c r="E72" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="34">
-        <v>3</v>
-      </c>
-      <c r="E46" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F46" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="41"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="40"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40"/>
-    </row>
-    <row r="48" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="49" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="63" t="s">
-        <v>41</v>
-      </c>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
-    </row>
-    <row r="50" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G50" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H50" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B51" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D51" s="2">
-        <v>50</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D52" s="6">
-        <v>50</v>
-      </c>
-      <c r="E52" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="51"/>
-      <c r="C53" s="50"/>
-      <c r="D53" s="50"/>
-      <c r="E53" s="50"/>
-      <c r="F53" s="50"/>
-      <c r="G53" s="50"/>
-      <c r="H53" s="50"/>
-    </row>
-    <row r="54" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="59"/>
-    </row>
-    <row r="55" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D55" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E55" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G55" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B56" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C56" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D56" s="28">
-        <v>50</v>
-      </c>
-      <c r="E56" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="F56" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H56" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D57" s="31">
-        <v>100</v>
-      </c>
-      <c r="E57" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H57" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="C58" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="D58" s="34">
-        <v>3</v>
-      </c>
-      <c r="E58" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="F58" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G58" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="60" t="s">
+      <c r="F72" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G72" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B75" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="C61" s="61"/>
-      <c r="D61" s="61"/>
-      <c r="E61" s="61"/>
-      <c r="F61" s="61"/>
-      <c r="G61" s="61"/>
-      <c r="H61" s="62"/>
-    </row>
-    <row r="62" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C62" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="G62" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H62" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="63" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="36" t="s">
-        <v>28</v>
-      </c>
-      <c r="C63" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="38">
-        <v>50</v>
-      </c>
-      <c r="E63" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F63" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G63" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H63" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="41"/>
-      <c r="C64" s="40"/>
-      <c r="D64" s="40"/>
-      <c r="E64" s="40"/>
-      <c r="F64" s="40"/>
-      <c r="G64" s="40"/>
-      <c r="H64" s="40"/>
-    </row>
-    <row r="65" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B65" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="58"/>
-      <c r="D65" s="58"/>
-      <c r="E65" s="58"/>
-      <c r="F65" s="58"/>
-      <c r="G65" s="58"/>
-      <c r="H65" s="59"/>
-    </row>
-    <row r="66" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C66" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G66" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H66" s="26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B67" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C67" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D67" s="28">
-        <v>50</v>
-      </c>
-      <c r="E67" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F67" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G67" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H67" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="D68" s="34">
-        <v>50</v>
-      </c>
-      <c r="E68" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F68" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G68" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H68" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B70" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C70" s="58"/>
-      <c r="D70" s="58"/>
-      <c r="E70" s="58"/>
-      <c r="F70" s="58"/>
-      <c r="G70" s="58"/>
-      <c r="H70" s="59"/>
-    </row>
-    <row r="71" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B71" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="C71" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="D71" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="E71" s="26" t="s">
-        <v>4</v>
-      </c>
-      <c r="F71" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="G71" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="H71" s="26" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="C72" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="D72" s="28">
-        <v>2</v>
-      </c>
-      <c r="E72" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F72" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G72" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H72" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="C73" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="D73" s="34">
-        <v>50</v>
-      </c>
-      <c r="E73" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="F73" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G73" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H73" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="60" t="s">
-        <v>63</v>
-      </c>
-      <c r="C75" s="61"/>
-      <c r="D75" s="61"/>
-      <c r="E75" s="61"/>
-      <c r="F75" s="61"/>
-      <c r="G75" s="61"/>
-      <c r="H75" s="62"/>
+      <c r="C75" s="69"/>
+      <c r="D75" s="69"/>
+      <c r="E75" s="69"/>
+      <c r="F75" s="69"/>
+      <c r="G75" s="69"/>
+      <c r="H75" s="70"/>
     </row>
     <row r="76" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="17" t="s">
@@ -2595,89 +2682,319 @@
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="14" t="s">
+    <row r="77" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C77" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="38">
+        <v>50</v>
+      </c>
+      <c r="E77" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="F77" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G77" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H77" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="41"/>
+      <c r="C78" s="40"/>
+      <c r="D78" s="40"/>
+      <c r="E78" s="40"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="40"/>
+      <c r="H78" s="40"/>
+    </row>
+    <row r="79" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B79" s="65" t="s">
+        <v>42</v>
+      </c>
+      <c r="C79" s="66"/>
+      <c r="D79" s="66"/>
+      <c r="E79" s="66"/>
+      <c r="F79" s="66"/>
+      <c r="G79" s="66"/>
+      <c r="H79" s="67"/>
+    </row>
+    <row r="80" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C80" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E80" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F80" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G80" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H80" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="28">
+        <v>50</v>
+      </c>
+      <c r="E81" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="F81" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="82" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="C82" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D82" s="34">
+        <v>50</v>
+      </c>
+      <c r="E82" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F82" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G82" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H82" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B84" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C77" s="8" t="s">
+      <c r="C84" s="66"/>
+      <c r="D84" s="66"/>
+      <c r="E84" s="66"/>
+      <c r="F84" s="66"/>
+      <c r="G84" s="66"/>
+      <c r="H84" s="67"/>
+    </row>
+    <row r="85" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C85" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="D85" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E85" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G85" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H85" s="26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B86" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D86" s="28">
+        <v>2</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G86" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B87" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D87" s="34">
+        <v>50</v>
+      </c>
+      <c r="E87" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="F87" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B89" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C89" s="69"/>
+      <c r="D89" s="69"/>
+      <c r="E89" s="69"/>
+      <c r="F89" s="69"/>
+      <c r="G89" s="69"/>
+      <c r="H89" s="70"/>
+    </row>
+    <row r="90" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E90" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="F90" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E77" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G77" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="46" t="s">
-        <v>54</v>
-      </c>
-      <c r="C78" s="47" t="s">
+      <c r="G90" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H90" s="17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D78" s="48">
+      <c r="D91" s="2">
+        <v>5</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B92" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D92" s="48">
         <v>2</v>
       </c>
-      <c r="E78" s="48" t="s">
-        <v>45</v>
-      </c>
-      <c r="F78" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G78" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="H78" s="49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="15" t="s">
+      <c r="E92" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F92" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G92" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" s="49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C93" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D93" s="6">
         <v>100</v>
       </c>
-      <c r="E79" s="6" t="s">
+      <c r="E93" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G79" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H79" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="F93" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B49:H49"/>
+  <mergeCells count="13">
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B89:H89"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B75:H75"/>
+    <mergeCell ref="B63:H63"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B22:H22"/>
     <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B38:H38"/>
-    <mergeCell ref="B42:H42"/>
-    <mergeCell ref="B54:H54"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B70:H70"/>
-    <mergeCell ref="B65:H65"/>
-    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="B52:H52"/>
+    <mergeCell ref="B56:H56"/>
+    <mergeCell ref="B36:H36"/>
+    <mergeCell ref="B44:H44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add diccionario de datos los cambios
</commit_message>
<xml_diff>
--- a/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
+++ b/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablofernandezsato/Desktop/Git/Libreriav2/DIAGRAMAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FEDE44-2DBC-7043-AEC4-DA7628FFD65B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505C0FED-473F-CF42-B1A8-21B056FD948C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35640" yWindow="1260" windowWidth="25440" windowHeight="14040" xr2:uid="{E2514F55-DB76-7447-8476-23FD56A879E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="65">
   <si>
     <t>LIBRO</t>
   </si>
@@ -222,16 +222,13 @@
     <t>LIBRO_BALDA</t>
   </si>
   <si>
-    <t>ESCRITOR</t>
-  </si>
-  <si>
-    <t>LIBRO_ESCRITOR</t>
-  </si>
-  <si>
     <t>LIBRO_ESCRITOR_DIBUJANTE</t>
   </si>
   <si>
     <t>ALIAS DEL DIBUJANTE</t>
+  </si>
+  <si>
+    <t>LIBRO_AUTOR</t>
   </si>
 </sst>
 </file>
@@ -876,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1065,79 +1062,97 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1454,10 +1469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896DC84-666B-2C40-BFB0-FA171D076670}">
-  <dimension ref="B5:H94"/>
+  <dimension ref="B5:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1468,15 +1483,15 @@
   <sheetData>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:8" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
+      <c r="C6" s="87"/>
+      <c r="D6" s="87"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="87"/>
     </row>
     <row r="7" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
@@ -1800,15 +1815,15 @@
     </row>
     <row r="21" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="64" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="64"/>
-      <c r="H22" s="64"/>
+      <c r="B22" s="87" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="87"/>
+      <c r="D22" s="87"/>
+      <c r="E22" s="87"/>
+      <c r="F22" s="87"/>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
     </row>
     <row r="23" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
@@ -1879,1122 +1894,1145 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="4">
         <v>50</v>
       </c>
-      <c r="E26" s="6" t="s">
+      <c r="E26" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="64"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-    </row>
-    <row r="29" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+      <c r="F26" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="91" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="90">
+        <v>50</v>
+      </c>
+      <c r="E27" s="90" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="90" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="90" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="89" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="87" t="s">
+        <v>25</v>
+      </c>
+      <c r="C29" s="87"/>
+      <c r="D29" s="87"/>
+      <c r="E29" s="87"/>
+      <c r="F29" s="87"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="87"/>
+    </row>
+    <row r="30" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C30" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D30" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E29" s="17" t="s">
+      <c r="E30" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="17" t="s">
+      <c r="F30" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G30" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H30" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="11" t="s">
+    <row r="31" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C31" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D31" s="2">
         <v>50</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="4">
-        <v>100</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H31" s="5" t="s">
+      <c r="F31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C32" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="4">
+        <v>100</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="4">
         <v>50</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="E33" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="13" t="s">
+      <c r="F33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C34" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6" t="s">
+      <c r="D34" s="6"/>
+      <c r="E34" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="64" t="s">
+      <c r="F34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-      <c r="F36" s="64"/>
-      <c r="G36" s="64"/>
-      <c r="H36" s="64"/>
-    </row>
-    <row r="37" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
+      <c r="C37" s="87"/>
+      <c r="D37" s="87"/>
+      <c r="E37" s="87"/>
+      <c r="F37" s="87"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="87"/>
+    </row>
+    <row r="38" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="17" t="s">
+      <c r="C38" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D38" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="17" t="s">
+      <c r="E38" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="17" t="s">
+      <c r="F38" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G38" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="11" t="s">
+    <row r="39" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C39" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D39" s="2">
         <v>50</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="4">
-        <v>100</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="5" t="s">
+      <c r="F39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B40" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D40" s="4">
+        <v>100</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="4">
         <v>50</v>
       </c>
-      <c r="E40" s="4" t="s">
+      <c r="E41" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="13" t="s">
+      <c r="F41" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="G41" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C41" s="10" t="s">
+      <c r="C42" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6" t="s">
+      <c r="D42" s="6"/>
+      <c r="E42" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H41" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="71"/>
-      <c r="D44" s="71"/>
-      <c r="E44" s="71"/>
-      <c r="F44" s="71"/>
-      <c r="G44" s="71"/>
-      <c r="H44" s="71"/>
-    </row>
-    <row r="45" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="72" t="s">
+      <c r="F42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="88" t="s">
+        <v>62</v>
+      </c>
+      <c r="C45" s="88"/>
+      <c r="D45" s="88"/>
+      <c r="E45" s="88"/>
+      <c r="F45" s="88"/>
+      <c r="G45" s="88"/>
+      <c r="H45" s="88"/>
+    </row>
+    <row r="46" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C45" s="72" t="s">
+      <c r="C46" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="72" t="s">
+      <c r="D46" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="72" t="s">
+      <c r="E46" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="72" t="s">
+      <c r="F46" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="G45" s="72" t="s">
+      <c r="G46" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="H45" s="72" t="s">
+      <c r="H46" s="64" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="73" t="s">
+    <row r="47" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="C46" s="74" t="s">
+      <c r="C47" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="D46" s="75">
+      <c r="D47" s="67">
         <v>5</v>
       </c>
-      <c r="E46" s="75" t="s">
+      <c r="E47" s="67" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="G46" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="76" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="77" t="s">
+      <c r="F47" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="68" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C47" s="78" t="s">
+      <c r="C48" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="79">
+      <c r="D48" s="71">
         <v>100</v>
       </c>
-      <c r="E47" s="79" t="s">
+      <c r="E48" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="F47" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="H47" s="80" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="81" t="s">
+      <c r="F48" s="71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="71" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="72" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="C48" s="82" t="s">
+      <c r="C49" s="74" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="83">
+      <c r="D49" s="75">
         <v>50</v>
       </c>
-      <c r="E48" s="83" t="s">
+      <c r="E49" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="F48" s="83" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="83" t="s">
-        <v>17</v>
-      </c>
-      <c r="H48" s="84" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="85" t="s">
+      <c r="F49" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="75" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C49" s="86" t="s">
+      <c r="C50" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="87">
+      <c r="D50" s="79">
         <v>50</v>
       </c>
-      <c r="E49" s="87" t="s">
-        <v>65</v>
-      </c>
-      <c r="F49" s="87" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="87" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="88" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="51" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="68" t="s">
+      <c r="E50" s="79" t="s">
+        <v>63</v>
+      </c>
+      <c r="F50" s="79" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="79" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="80" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="52" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="69"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="69"/>
-      <c r="F52" s="69"/>
-      <c r="G52" s="69"/>
-      <c r="H52" s="70"/>
-    </row>
-    <row r="53" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="17" t="s">
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="86"/>
+    </row>
+    <row r="54" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C53" s="17" t="s">
+      <c r="C54" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D54" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="E54" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F54" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G54" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H54" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="36" t="s">
+    <row r="55" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C55" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D54" s="38">
+      <c r="D55" s="38">
         <v>50</v>
       </c>
-      <c r="E54" s="38" t="s">
+      <c r="E55" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="F54" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G54" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H54" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="65" t="s">
+      <c r="F55" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="C56" s="66"/>
-      <c r="D56" s="66"/>
-      <c r="E56" s="66"/>
-      <c r="F56" s="66"/>
-      <c r="G56" s="66"/>
-      <c r="H56" s="67"/>
-    </row>
-    <row r="57" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="25" t="s">
+      <c r="C57" s="82"/>
+      <c r="D57" s="82"/>
+      <c r="E57" s="82"/>
+      <c r="F57" s="82"/>
+      <c r="G57" s="82"/>
+      <c r="H57" s="83"/>
+    </row>
+    <row r="58" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="C58" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="26" t="s">
+      <c r="D58" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E57" s="26" t="s">
+      <c r="E58" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="26" t="s">
+      <c r="F58" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G57" s="26" t="s">
+      <c r="G58" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="26" t="s">
+      <c r="H58" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B58" s="27" t="s">
+    <row r="59" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C59" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="28">
+      <c r="D59" s="28">
         <v>50</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E59" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F58" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="30" t="s">
+      <c r="F59" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C59" s="31" t="s">
+      <c r="C60" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="31">
+      <c r="D60" s="31">
         <v>100</v>
       </c>
-      <c r="E59" s="31" t="s">
+      <c r="E60" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F59" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H59" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="33" t="s">
+      <c r="F60" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C60" s="34" t="s">
+      <c r="C61" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="34">
+      <c r="D61" s="34">
         <v>3</v>
       </c>
-      <c r="E60" s="34" t="s">
+      <c r="E61" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F60" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G60" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H60" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B61" s="41"/>
-      <c r="C61" s="40"/>
-      <c r="D61" s="40"/>
-      <c r="E61" s="40"/>
-      <c r="F61" s="40"/>
-      <c r="G61" s="40"/>
-      <c r="H61" s="40"/>
-    </row>
-    <row r="62" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="64" t="s">
+      <c r="F61" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="41"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
+      <c r="F62" s="40"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="40"/>
+    </row>
+    <row r="63" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="87" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="64"/>
-      <c r="D63" s="64"/>
-      <c r="E63" s="64"/>
-      <c r="F63" s="64"/>
-      <c r="G63" s="64"/>
-      <c r="H63" s="64"/>
-    </row>
-    <row r="64" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="17" t="s">
+      <c r="C64" s="87"/>
+      <c r="D64" s="87"/>
+      <c r="E64" s="87"/>
+      <c r="F64" s="87"/>
+      <c r="G64" s="87"/>
+      <c r="H64" s="87"/>
+    </row>
+    <row r="65" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C64" s="17" t="s">
+      <c r="C65" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D64" s="17" t="s">
+      <c r="D65" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E64" s="17" t="s">
+      <c r="E65" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F64" s="17" t="s">
+      <c r="F65" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G65" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H64" s="17" t="s">
+      <c r="H65" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="11" t="s">
+    <row r="66" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C66" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D66" s="2">
         <v>50</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="E66" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="13" t="s">
+      <c r="F66" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C66" s="10" t="s">
+      <c r="C67" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D66" s="6">
+      <c r="D67" s="6">
         <v>50</v>
       </c>
-      <c r="E66" s="6" t="s">
+      <c r="E67" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F66" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H66" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="51"/>
-      <c r="C67" s="50"/>
-      <c r="D67" s="50"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50"/>
-    </row>
-    <row r="68" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B68" s="65" t="s">
+      <c r="F67" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="51"/>
+      <c r="C68" s="50"/>
+      <c r="D68" s="50"/>
+      <c r="E68" s="50"/>
+      <c r="F68" s="50"/>
+      <c r="G68" s="50"/>
+      <c r="H68" s="50"/>
+    </row>
+    <row r="69" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B69" s="81" t="s">
         <v>49</v>
       </c>
-      <c r="C68" s="66"/>
-      <c r="D68" s="66"/>
-      <c r="E68" s="66"/>
-      <c r="F68" s="66"/>
-      <c r="G68" s="66"/>
-      <c r="H68" s="67"/>
-    </row>
-    <row r="69" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="25" t="s">
+      <c r="C69" s="82"/>
+      <c r="D69" s="82"/>
+      <c r="E69" s="82"/>
+      <c r="F69" s="82"/>
+      <c r="G69" s="82"/>
+      <c r="H69" s="83"/>
+    </row>
+    <row r="70" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="26" t="s">
+      <c r="C70" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D69" s="26" t="s">
+      <c r="D70" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="26" t="s">
+      <c r="E70" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F69" s="26" t="s">
+      <c r="F70" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G69" s="26" t="s">
+      <c r="G70" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H69" s="26" t="s">
+      <c r="H70" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B70" s="27" t="s">
+    <row r="71" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="C70" s="28" t="s">
+      <c r="C71" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D70" s="28">
+      <c r="D71" s="28">
         <v>50</v>
       </c>
-      <c r="E70" s="28" t="s">
+      <c r="E71" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="F70" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G70" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H70" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B71" s="30" t="s">
+      <c r="F71" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B72" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C71" s="31" t="s">
+      <c r="C72" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D71" s="31">
+      <c r="D72" s="31">
         <v>100</v>
       </c>
-      <c r="E71" s="31" t="s">
+      <c r="E72" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="F71" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H71" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="72" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="33" t="s">
+      <c r="F72" s="31" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C72" s="34" t="s">
+      <c r="C73" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D72" s="34">
+      <c r="D73" s="34">
         <v>3</v>
       </c>
-      <c r="E72" s="34" t="s">
+      <c r="E73" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F72" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G72" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H72" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="68" t="s">
+      <c r="F73" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B76" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="69"/>
-      <c r="D75" s="69"/>
-      <c r="E75" s="69"/>
-      <c r="F75" s="69"/>
-      <c r="G75" s="69"/>
-      <c r="H75" s="70"/>
-    </row>
-    <row r="76" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="17" t="s">
+      <c r="C76" s="85"/>
+      <c r="D76" s="85"/>
+      <c r="E76" s="85"/>
+      <c r="F76" s="85"/>
+      <c r="G76" s="85"/>
+      <c r="H76" s="86"/>
+    </row>
+    <row r="77" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C76" s="17" t="s">
+      <c r="C77" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D76" s="17" t="s">
+      <c r="D77" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E76" s="17" t="s">
+      <c r="E77" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F76" s="17" t="s">
+      <c r="F77" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G76" s="17" t="s">
+      <c r="G77" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H76" s="17" t="s">
+      <c r="H77" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="77" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="36" t="s">
+    <row r="78" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="37" t="s">
+      <c r="C78" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D77" s="38">
+      <c r="D78" s="38">
         <v>50</v>
       </c>
-      <c r="E77" s="38" t="s">
+      <c r="E78" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="F77" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G77" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H77" s="39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="41"/>
-      <c r="C78" s="40"/>
-      <c r="D78" s="40"/>
-      <c r="E78" s="40"/>
-      <c r="F78" s="40"/>
-      <c r="G78" s="40"/>
-      <c r="H78" s="40"/>
-    </row>
-    <row r="79" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B79" s="65" t="s">
+      <c r="F78" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" s="39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="41"/>
+      <c r="C79" s="40"/>
+      <c r="D79" s="40"/>
+      <c r="E79" s="40"/>
+      <c r="F79" s="40"/>
+      <c r="G79" s="40"/>
+      <c r="H79" s="40"/>
+    </row>
+    <row r="80" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B80" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="C79" s="66"/>
-      <c r="D79" s="66"/>
-      <c r="E79" s="66"/>
-      <c r="F79" s="66"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="67"/>
-    </row>
-    <row r="80" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="25" t="s">
+      <c r="C80" s="82"/>
+      <c r="D80" s="82"/>
+      <c r="E80" s="82"/>
+      <c r="F80" s="82"/>
+      <c r="G80" s="82"/>
+      <c r="H80" s="83"/>
+    </row>
+    <row r="81" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C80" s="26" t="s">
+      <c r="C81" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D80" s="26" t="s">
+      <c r="D81" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E80" s="26" t="s">
+      <c r="E81" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F80" s="26" t="s">
+      <c r="F81" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G80" s="26" t="s">
+      <c r="G81" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H80" s="26" t="s">
+      <c r="H81" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B81" s="27" t="s">
+    <row r="82" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C81" s="28" t="s">
+      <c r="C82" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D81" s="28">
+      <c r="D82" s="28">
         <v>50</v>
       </c>
-      <c r="E81" s="28" t="s">
+      <c r="E82" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F81" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G81" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H81" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="82" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="33" t="s">
+      <c r="F82" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C82" s="34" t="s">
+      <c r="C83" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="34">
+      <c r="D83" s="34">
         <v>50</v>
       </c>
-      <c r="E82" s="34" t="s">
+      <c r="E83" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="F82" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G82" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H82" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="83" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="84" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="65" t="s">
+      <c r="F83" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="84" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B85" s="81" t="s">
         <v>53</v>
       </c>
-      <c r="C84" s="66"/>
-      <c r="D84" s="66"/>
-      <c r="E84" s="66"/>
-      <c r="F84" s="66"/>
-      <c r="G84" s="66"/>
-      <c r="H84" s="67"/>
-    </row>
-    <row r="85" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B85" s="25" t="s">
+      <c r="C85" s="82"/>
+      <c r="D85" s="82"/>
+      <c r="E85" s="82"/>
+      <c r="F85" s="82"/>
+      <c r="G85" s="82"/>
+      <c r="H85" s="83"/>
+    </row>
+    <row r="86" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C85" s="26" t="s">
+      <c r="C86" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D85" s="26" t="s">
+      <c r="D86" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="E85" s="26" t="s">
+      <c r="E86" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="F85" s="26" t="s">
+      <c r="F86" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="G85" s="26" t="s">
+      <c r="G86" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="H85" s="26" t="s">
+      <c r="H86" s="26" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="86" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B86" s="27" t="s">
+    <row r="87" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C86" s="28" t="s">
+      <c r="C87" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="D86" s="28">
+      <c r="D87" s="28">
         <v>2</v>
       </c>
-      <c r="E86" s="28" t="s">
+      <c r="E87" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="F86" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G86" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H86" s="29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B87" s="33" t="s">
+      <c r="F87" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="88" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C87" s="34" t="s">
+      <c r="C88" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="D87" s="34">
+      <c r="D88" s="34">
         <v>50</v>
       </c>
-      <c r="E87" s="34" t="s">
+      <c r="E88" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="F87" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G87" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="35" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="89" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="68" t="s">
+      <c r="F88" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B90" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="C89" s="69"/>
-      <c r="D89" s="69"/>
-      <c r="E89" s="69"/>
-      <c r="F89" s="69"/>
-      <c r="G89" s="69"/>
-      <c r="H89" s="70"/>
-    </row>
-    <row r="90" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="17" t="s">
+      <c r="C90" s="85"/>
+      <c r="D90" s="85"/>
+      <c r="E90" s="85"/>
+      <c r="F90" s="85"/>
+      <c r="G90" s="85"/>
+      <c r="H90" s="86"/>
+    </row>
+    <row r="91" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C90" s="17" t="s">
+      <c r="C91" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="D90" s="17" t="s">
+      <c r="D91" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E90" s="17" t="s">
+      <c r="E91" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="17" t="s">
+      <c r="F91" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G90" s="17" t="s">
+      <c r="G91" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H90" s="17" t="s">
+      <c r="H91" s="17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="91" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="14" t="s">
+    <row r="92" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C91" s="8" t="s">
+      <c r="C92" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D92" s="2">
         <v>5</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F91" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G91" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="46" t="s">
+      <c r="F92" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B93" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C92" s="47" t="s">
+      <c r="C93" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="48">
+      <c r="D93" s="48">
         <v>2</v>
       </c>
-      <c r="E92" s="48" t="s">
+      <c r="E93" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="F92" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G92" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="H92" s="49" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="93" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="15" t="s">
+      <c r="F93" s="48" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="49" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C94" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D94" s="6">
         <v>100</v>
       </c>
-      <c r="E93" s="6" t="s">
+      <c r="E94" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F93" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G93" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="94" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+      <c r="F94" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G94" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="95" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B89:H89"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B75:H75"/>
-    <mergeCell ref="B63:H63"/>
+    <mergeCell ref="B64:H64"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="B52:H52"/>
-    <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B36:H36"/>
-    <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B29:H29"/>
+    <mergeCell ref="B53:H53"/>
+    <mergeCell ref="B57:H57"/>
+    <mergeCell ref="B37:H37"/>
+    <mergeCell ref="B45:H45"/>
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B76:H76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correccion en diccionario de datos
</commit_message>
<xml_diff>
--- a/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
+++ b/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablofernandezsato/Desktop/Git/Libreriav2/DIAGRAMAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{505C0FED-473F-CF42-B1A8-21B056FD948C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD124E39-FD5F-2D41-A8FC-F3D7AF9FA62E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35640" yWindow="1260" windowWidth="25440" windowHeight="14040" xr2:uid="{E2514F55-DB76-7447-8476-23FD56A879E1}"/>
   </bookViews>
@@ -168,9 +168,6 @@
     <t>NOMBRE DE LA ESTANTERIA</t>
   </si>
   <si>
-    <t>NUMERO DE VALDA</t>
-  </si>
-  <si>
     <t>INDICE DEL LIBRO</t>
   </si>
   <si>
@@ -180,9 +177,6 @@
     <t>ESTANTERIA DONDE ESTÁ</t>
   </si>
   <si>
-    <t>INDICE DE LA VALDA</t>
-  </si>
-  <si>
     <t>SAGA_VOLUMEN</t>
   </si>
   <si>
@@ -229,6 +223,12 @@
   </si>
   <si>
     <t>LIBRO_AUTOR</t>
+  </si>
+  <si>
+    <t>INDICE DE LA BALDA</t>
+  </si>
+  <si>
+    <t>NUMERO DE BALDA</t>
   </si>
 </sst>
 </file>
@@ -873,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -917,9 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1113,6 +1110,36 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1122,37 +1149,28 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1471,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896DC84-666B-2C40-BFB0-FA171D076670}">
   <dimension ref="B5:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1483,90 +1501,90 @@
   <sheetData>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:8" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
     </row>
     <row r="7" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="16" t="s">
+      <c r="H7" s="15" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="19">
+        <v>5</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="20">
-        <v>5</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="21" t="s">
+      <c r="F8" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="44">
+      <c r="D9" s="43">
         <v>100</v>
       </c>
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="45" t="s">
+      <c r="F9" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="22" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="1">
@@ -1581,15 +1599,15 @@
       <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="1">
@@ -1604,15 +1622,15 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1">
@@ -1627,20 +1645,20 @@
       <c r="G12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>18</v>
@@ -1648,22 +1666,22 @@
       <c r="G13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="23" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="1">
         <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>18</v>
@@ -1671,22 +1689,22 @@
       <c r="G14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D15" s="1">
         <v>50</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>18</v>
@@ -1694,15 +1712,15 @@
       <c r="G15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="22" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="1">
@@ -1717,140 +1735,140 @@
       <c r="G16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
+      <c r="H16" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="58" t="s">
+      <c r="C17" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="59">
+      <c r="D17" s="58">
         <v>3</v>
       </c>
-      <c r="E17" s="59" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" s="56" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="58" t="s">
+      <c r="E17" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="55" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="59">
+      <c r="D18" s="58">
         <v>2</v>
       </c>
-      <c r="E18" s="59" t="s">
+      <c r="E18" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="58" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="59" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="53">
+        <v>3</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="54" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="61">
+        <v>3</v>
+      </c>
+      <c r="E20" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="59" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="59" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="60" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="53" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="54">
-        <v>3</v>
-      </c>
-      <c r="E19" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="F19" s="54" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="55" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="61" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="62">
-        <v>3</v>
-      </c>
-      <c r="E20" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="62" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="63" t="s">
+      <c r="F20" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="62" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="87" t="s">
-        <v>64</v>
-      </c>
-      <c r="C22" s="87"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="87"/>
-      <c r="F22" s="87"/>
-      <c r="G22" s="87"/>
-      <c r="H22" s="87"/>
+      <c r="B22" s="86" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="86"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="86"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="86"/>
     </row>
     <row r="23" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="17" t="s">
+      <c r="E23" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F23" s="17" t="s">
+      <c r="F23" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B24" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>20</v>
@@ -1859,7 +1877,7 @@
         <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>17</v>
@@ -1872,33 +1890,33 @@
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="47" t="s">
+      <c r="C25" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="48">
+      <c r="D25" s="47">
         <v>100</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="F25" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="49" t="s">
+      <c r="F25" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="48" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="94" t="s">
+      <c r="B26" s="85" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="92" t="s">
+      <c r="C26" s="83" t="s">
         <v>15</v>
       </c>
       <c r="D26" s="4">
@@ -1918,60 +1936,60 @@
       </c>
     </row>
     <row r="27" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="93" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="91" t="s">
+      <c r="B27" s="84" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="90">
+      <c r="D27" s="81">
         <v>50</v>
       </c>
-      <c r="E27" s="90" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="90" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="H27" s="89" t="s">
+      <c r="E27" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="F27" s="81" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="81" t="s">
+        <v>17</v>
+      </c>
+      <c r="H27" s="80" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="87" t="s">
+      <c r="B29" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="87"/>
-      <c r="D29" s="87"/>
-      <c r="E29" s="87"/>
-      <c r="F29" s="87"/>
-      <c r="G29" s="87"/>
-      <c r="H29" s="87"/>
+      <c r="C29" s="86"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
+      <c r="G29" s="86"/>
+      <c r="H29" s="86"/>
     </row>
     <row r="30" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D30" s="17" t="s">
+      <c r="D30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="H30" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2068,36 +2086,36 @@
     <row r="35" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="37" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="C37" s="87"/>
-      <c r="D37" s="87"/>
-      <c r="E37" s="87"/>
-      <c r="F37" s="87"/>
-      <c r="G37" s="87"/>
-      <c r="H37" s="87"/>
+      <c r="B37" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="86"/>
+      <c r="D37" s="86"/>
+      <c r="E37" s="86"/>
+      <c r="F37" s="86"/>
+      <c r="G37" s="86"/>
+      <c r="H37" s="86"/>
     </row>
     <row r="38" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="17" t="s">
+      <c r="C38" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="G38" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2194,335 +2212,335 @@
     <row r="43" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="88"/>
-      <c r="D45" s="88"/>
-      <c r="E45" s="88"/>
-      <c r="F45" s="88"/>
-      <c r="G45" s="88"/>
-      <c r="H45" s="88"/>
+      <c r="B45" s="93" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="93"/>
+      <c r="D45" s="93"/>
+      <c r="E45" s="93"/>
+      <c r="F45" s="93"/>
+      <c r="G45" s="93"/>
+      <c r="H45" s="93"/>
     </row>
     <row r="46" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C46" s="64" t="s">
+      <c r="C46" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D46" s="64" t="s">
+      <c r="D46" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E46" s="64" t="s">
+      <c r="E46" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="64" t="s">
+      <c r="F46" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G46" s="64" t="s">
+      <c r="G46" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H46" s="64" t="s">
+      <c r="H46" s="63" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="47" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B47" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="C47" s="66" t="s">
+      <c r="B47" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D47" s="67">
+      <c r="D47" s="66">
         <v>5</v>
       </c>
-      <c r="E47" s="67" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="67" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="67" t="s">
-        <v>18</v>
-      </c>
-      <c r="H47" s="68" t="s">
+      <c r="E47" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H47" s="67" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="C48" s="70" t="s">
+      <c r="C48" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="71">
+      <c r="D48" s="70">
         <v>100</v>
       </c>
-      <c r="E48" s="71" t="s">
+      <c r="E48" s="70" t="s">
         <v>16</v>
       </c>
-      <c r="F48" s="71" t="s">
-        <v>18</v>
-      </c>
-      <c r="G48" s="71" t="s">
-        <v>17</v>
-      </c>
-      <c r="H48" s="72" t="s">
+      <c r="F48" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G48" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H48" s="71" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="73" t="s">
+      <c r="B49" s="72" t="s">
         <v>25</v>
       </c>
-      <c r="C49" s="74" t="s">
+      <c r="C49" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="75">
+      <c r="D49" s="74">
         <v>50</v>
       </c>
-      <c r="E49" s="75" t="s">
+      <c r="E49" s="74" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="75" t="s">
-        <v>18</v>
-      </c>
-      <c r="G49" s="75" t="s">
-        <v>17</v>
-      </c>
-      <c r="H49" s="76" t="s">
+      <c r="F49" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="G49" s="74" t="s">
+        <v>17</v>
+      </c>
+      <c r="H49" s="75" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="50" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="C50" s="78" t="s">
+      <c r="B50" s="76" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D50" s="79">
+      <c r="D50" s="78">
         <v>50</v>
       </c>
-      <c r="E50" s="79" t="s">
-        <v>63</v>
-      </c>
-      <c r="F50" s="79" t="s">
-        <v>18</v>
-      </c>
-      <c r="G50" s="79" t="s">
-        <v>17</v>
-      </c>
-      <c r="H50" s="80" t="s">
+      <c r="E50" s="78" t="s">
+        <v>61</v>
+      </c>
+      <c r="F50" s="78" t="s">
+        <v>18</v>
+      </c>
+      <c r="G50" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="H50" s="79" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="51" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="52" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="84" t="s">
+      <c r="B53" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="85"/>
-      <c r="D53" s="85"/>
-      <c r="E53" s="85"/>
-      <c r="F53" s="85"/>
-      <c r="G53" s="85"/>
-      <c r="H53" s="86"/>
+      <c r="C53" s="88"/>
+      <c r="D53" s="88"/>
+      <c r="E53" s="88"/>
+      <c r="F53" s="88"/>
+      <c r="G53" s="88"/>
+      <c r="H53" s="89"/>
     </row>
     <row r="54" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C54" s="17" t="s">
+      <c r="C54" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G54" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H54" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="55" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="36" t="s">
+      <c r="B55" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C55" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D55" s="38">
+      <c r="D55" s="37">
         <v>50</v>
       </c>
-      <c r="E55" s="38" t="s">
+      <c r="E55" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="F55" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G55" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H55" s="39" t="s">
+      <c r="F55" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G55" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H55" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="56" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="81" t="s">
+      <c r="B57" s="90" t="s">
         <v>37</v>
       </c>
-      <c r="C57" s="82"/>
-      <c r="D57" s="82"/>
-      <c r="E57" s="82"/>
-      <c r="F57" s="82"/>
-      <c r="G57" s="82"/>
-      <c r="H57" s="83"/>
+      <c r="C57" s="91"/>
+      <c r="D57" s="91"/>
+      <c r="E57" s="91"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
+      <c r="H57" s="92"/>
     </row>
     <row r="58" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="25" t="s">
+      <c r="B58" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="26" t="s">
+      <c r="C58" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D58" s="26" t="s">
+      <c r="D58" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="26" t="s">
+      <c r="E58" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="26" t="s">
+      <c r="F58" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G58" s="26" t="s">
+      <c r="G58" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H58" s="26" t="s">
+      <c r="H58" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="59" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D59" s="28">
+      <c r="D59" s="27">
         <v>50</v>
       </c>
-      <c r="E59" s="28" t="s">
+      <c r="E59" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F59" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H59" s="29" t="s">
+      <c r="F59" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G59" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H59" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C60" s="31" t="s">
+      <c r="C60" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="31">
+      <c r="D60" s="30">
         <v>100</v>
       </c>
-      <c r="E60" s="31" t="s">
+      <c r="E60" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F60" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H60" s="32" t="s">
+      <c r="F60" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="61" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="33" t="s">
+      <c r="B61" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C61" s="34" t="s">
+      <c r="C61" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="34">
+      <c r="D61" s="33">
         <v>3</v>
       </c>
-      <c r="E61" s="34" t="s">
+      <c r="E61" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F61" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H61" s="35" t="s">
+      <c r="F61" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H61" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B62" s="41"/>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="39"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="39"/>
+      <c r="H62" s="39"/>
     </row>
     <row r="63" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="87" t="s">
+      <c r="B64" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C64" s="87"/>
-      <c r="D64" s="87"/>
-      <c r="E64" s="87"/>
-      <c r="F64" s="87"/>
-      <c r="G64" s="87"/>
-      <c r="H64" s="87"/>
+      <c r="C64" s="86"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="86"/>
+      <c r="F64" s="86"/>
+      <c r="G64" s="86"/>
+      <c r="H64" s="86"/>
     </row>
     <row r="65" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C65" s="17" t="s">
+      <c r="C65" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D65" s="17" t="s">
+      <c r="D65" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="E65" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F65" s="17" t="s">
+      <c r="F65" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G65" s="17" t="s">
+      <c r="G65" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H65" s="17" t="s">
+      <c r="H65" s="16" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2573,453 +2591,458 @@
       </c>
     </row>
     <row r="68" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="51"/>
-      <c r="C68" s="50"/>
-      <c r="D68" s="50"/>
-      <c r="E68" s="50"/>
-      <c r="F68" s="50"/>
-      <c r="G68" s="50"/>
-      <c r="H68" s="50"/>
+      <c r="B68" s="50"/>
+      <c r="C68" s="49"/>
+      <c r="D68" s="49"/>
+      <c r="E68" s="49"/>
+      <c r="F68" s="49"/>
+      <c r="G68" s="49"/>
+      <c r="H68" s="49"/>
     </row>
     <row r="69" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="81" t="s">
-        <v>49</v>
-      </c>
-      <c r="C69" s="82"/>
-      <c r="D69" s="82"/>
-      <c r="E69" s="82"/>
-      <c r="F69" s="82"/>
-      <c r="G69" s="82"/>
-      <c r="H69" s="83"/>
+      <c r="B69" s="90" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" s="91"/>
+      <c r="D69" s="91"/>
+      <c r="E69" s="91"/>
+      <c r="F69" s="91"/>
+      <c r="G69" s="91"/>
+      <c r="H69" s="92"/>
     </row>
     <row r="70" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C70" s="26" t="s">
+      <c r="C70" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D70" s="26" t="s">
+      <c r="D70" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E70" s="26" t="s">
+      <c r="E70" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F70" s="26" t="s">
+      <c r="F70" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G70" s="26" t="s">
+      <c r="G70" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H70" s="26" t="s">
+      <c r="H70" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="71" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B71" s="27" t="s">
+      <c r="B71" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C71" s="28" t="s">
+      <c r="C71" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D71" s="28">
+      <c r="D71" s="27">
         <v>50</v>
       </c>
-      <c r="E71" s="28" t="s">
+      <c r="E71" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="F71" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="H71" s="29" t="s">
+      <c r="F71" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H71" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C72" s="31" t="s">
+      <c r="C72" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="D72" s="31">
+      <c r="D72" s="30">
         <v>100</v>
       </c>
-      <c r="E72" s="31" t="s">
+      <c r="E72" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="F72" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="G72" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="H72" s="32" t="s">
+      <c r="F72" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G72" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="H72" s="31" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="73" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="33" t="s">
+      <c r="B73" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="C73" s="34" t="s">
+      <c r="C73" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D73" s="34">
+      <c r="D73" s="33">
         <v>3</v>
       </c>
-      <c r="E73" s="34" t="s">
+      <c r="E73" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="F73" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="G73" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H73" s="35" t="s">
+      <c r="F73" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="G73" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H73" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="74" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="84" t="s">
+      <c r="B76" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="C76" s="85"/>
-      <c r="D76" s="85"/>
-      <c r="E76" s="85"/>
-      <c r="F76" s="85"/>
-      <c r="G76" s="85"/>
-      <c r="H76" s="86"/>
+      <c r="C76" s="88"/>
+      <c r="D76" s="88"/>
+      <c r="E76" s="88"/>
+      <c r="F76" s="88"/>
+      <c r="G76" s="88"/>
+      <c r="H76" s="89"/>
     </row>
     <row r="77" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C77" s="17" t="s">
+      <c r="C77" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D77" s="17" t="s">
+      <c r="D77" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E77" s="17" t="s">
+      <c r="E77" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="F77" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G77" s="17" t="s">
+      <c r="G77" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H77" s="17" t="s">
+      <c r="H77" s="16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B78" s="36" t="s">
+      <c r="B78" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C78" s="37" t="s">
+      <c r="C78" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D78" s="38">
+      <c r="D78" s="37">
         <v>50</v>
       </c>
-      <c r="E78" s="38" t="s">
+      <c r="E78" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="F78" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="G78" s="38" t="s">
-        <v>18</v>
-      </c>
-      <c r="H78" s="39" t="s">
+      <c r="F78" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G78" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78" s="38" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="79" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B79" s="41"/>
-      <c r="C79" s="40"/>
-      <c r="D79" s="40"/>
-      <c r="E79" s="40"/>
-      <c r="F79" s="40"/>
-      <c r="G79" s="40"/>
-      <c r="H79" s="40"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="39"/>
+      <c r="D79" s="39"/>
+      <c r="E79" s="39"/>
+      <c r="F79" s="39"/>
+      <c r="G79" s="39"/>
+      <c r="H79" s="39"/>
     </row>
     <row r="80" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B80" s="81" t="s">
+      <c r="B80" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="C80" s="82"/>
-      <c r="D80" s="82"/>
-      <c r="E80" s="82"/>
-      <c r="F80" s="82"/>
-      <c r="G80" s="82"/>
-      <c r="H80" s="83"/>
+      <c r="C80" s="91"/>
+      <c r="D80" s="91"/>
+      <c r="E80" s="91"/>
+      <c r="F80" s="91"/>
+      <c r="G80" s="91"/>
+      <c r="H80" s="92"/>
     </row>
     <row r="81" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B81" s="25" t="s">
+      <c r="B81" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C81" s="26" t="s">
+      <c r="C81" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D81" s="26" t="s">
+      <c r="D81" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E81" s="26" t="s">
+      <c r="E81" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="26" t="s">
+      <c r="F81" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G81" s="26" t="s">
+      <c r="G81" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H81" s="26" t="s">
+      <c r="H81" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="82" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B82" s="27" t="s">
+      <c r="B82" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C82" s="28" t="s">
+      <c r="C82" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D82" s="28">
+      <c r="D82" s="27">
         <v>50</v>
       </c>
-      <c r="E82" s="28" t="s">
+      <c r="E82" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F82" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G82" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H82" s="29" t="s">
+      <c r="F82" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G82" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="33" t="s">
+      <c r="B83" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="34" t="s">
+      <c r="C83" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D83" s="34">
+      <c r="D83" s="33">
         <v>50</v>
       </c>
-      <c r="E83" s="34" t="s">
+      <c r="E83" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="F83" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G83" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H83" s="35" t="s">
+      <c r="F83" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G83" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H83" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="84" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="85" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B85" s="81" t="s">
-        <v>53</v>
-      </c>
-      <c r="C85" s="82"/>
-      <c r="D85" s="82"/>
-      <c r="E85" s="82"/>
-      <c r="F85" s="82"/>
-      <c r="G85" s="82"/>
-      <c r="H85" s="83"/>
+      <c r="B85" s="90" t="s">
+        <v>51</v>
+      </c>
+      <c r="C85" s="91"/>
+      <c r="D85" s="91"/>
+      <c r="E85" s="91"/>
+      <c r="F85" s="91"/>
+      <c r="G85" s="91"/>
+      <c r="H85" s="92"/>
     </row>
     <row r="86" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B86" s="25" t="s">
+      <c r="B86" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C86" s="26" t="s">
+      <c r="C86" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D86" s="26" t="s">
+      <c r="D86" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E86" s="26" t="s">
+      <c r="E86" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F86" s="26" t="s">
+      <c r="F86" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G86" s="26" t="s">
+      <c r="G86" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H86" s="26" t="s">
+      <c r="H86" s="25" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="87" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B87" s="27" t="s">
+      <c r="B87" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C87" s="28" t="s">
+      <c r="C87" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="28">
+      <c r="D87" s="27">
         <v>2</v>
       </c>
-      <c r="E87" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F87" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="G87" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="H87" s="29" t="s">
+      <c r="E87" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F87" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="G87" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87" s="28" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="88" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="33" t="s">
+      <c r="B88" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="C88" s="34" t="s">
+      <c r="C88" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D88" s="34">
+      <c r="D88" s="33">
         <v>50</v>
       </c>
-      <c r="E88" s="34" t="s">
+      <c r="E88" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F88" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="G88" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="H88" s="35" t="s">
+      <c r="F88" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G88" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="34" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="89" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="84" t="s">
-        <v>61</v>
-      </c>
-      <c r="C90" s="85"/>
-      <c r="D90" s="85"/>
-      <c r="E90" s="85"/>
-      <c r="F90" s="85"/>
-      <c r="G90" s="85"/>
-      <c r="H90" s="86"/>
+      <c r="B90" s="94" t="s">
+        <v>59</v>
+      </c>
+      <c r="C90" s="95"/>
+      <c r="D90" s="95"/>
+      <c r="E90" s="95"/>
+      <c r="F90" s="95"/>
+      <c r="G90" s="95"/>
+      <c r="H90" s="96"/>
     </row>
     <row r="91" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="17" t="s">
+      <c r="C91" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="D91" s="17" t="s">
+      <c r="D91" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E91" s="17" t="s">
+      <c r="E91" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="F91" s="17" t="s">
+      <c r="F91" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="G91" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="H91" s="17" t="s">
+      <c r="H91" s="63" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="92" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C92" s="8" t="s">
+      <c r="B92" s="64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92" s="66">
         <v>5</v>
       </c>
-      <c r="E92" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F92" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H92" s="3" t="s">
+      <c r="E92" s="66" t="s">
+        <v>63</v>
+      </c>
+      <c r="F92" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="G92" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="H92" s="67" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="46" t="s">
-        <v>53</v>
-      </c>
-      <c r="C93" s="47" t="s">
+      <c r="B93" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="C93" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="D93" s="48">
+      <c r="D93" s="70">
         <v>2</v>
       </c>
-      <c r="E93" s="48" t="s">
-        <v>44</v>
-      </c>
-      <c r="F93" s="48" t="s">
-        <v>18</v>
-      </c>
-      <c r="G93" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="H93" s="49" t="s">
+      <c r="E93" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="F93" s="70" t="s">
+        <v>18</v>
+      </c>
+      <c r="G93" s="70" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="71" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="94" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="15" t="s">
+      <c r="B94" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" s="98" t="s">
         <v>15</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="99">
         <v>100</v>
       </c>
-      <c r="E94" s="6" t="s">
+      <c r="E94" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="F94" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G94" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="7" t="s">
+      <c r="F94" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="G94" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="100" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="95" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B69:H69"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B80:H80"/>
+    <mergeCell ref="B76:H76"/>
     <mergeCell ref="B64:H64"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B22:H22"/>
@@ -3028,11 +3051,6 @@
     <mergeCell ref="B57:H57"/>
     <mergeCell ref="B37:H37"/>
     <mergeCell ref="B45:H45"/>
-    <mergeCell ref="B69:H69"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="B80:H80"/>
-    <mergeCell ref="B76:H76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add tablas idioma y genero
</commit_message>
<xml_diff>
--- a/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
+++ b/DIAGRAMAS/DICCIONARIO DE DATOS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pablofernandezsato/Desktop/Git/Libreriav2/DIAGRAMAS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77AF2E09-1F72-B442-9913-614FC615653A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCE51B-FBAC-E142-B508-498C91B6B439}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35640" yWindow="1240" windowWidth="31940" windowHeight="19540" xr2:uid="{E2514F55-DB76-7447-8476-23FD56A879E1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="66">
   <si>
     <t>LIBRO</t>
   </si>
@@ -1170,50 +1170,50 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1534,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5896DC84-666B-2C40-BFB0-FA171D076670}">
-  <dimension ref="B5:H95"/>
+  <dimension ref="B5:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:H84"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1548,15 +1548,15 @@
   <sheetData>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="2:8" ht="20" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
+      <c r="C6" s="110"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="110"/>
+      <c r="H6" s="110"/>
     </row>
     <row r="7" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
@@ -1880,15 +1880,15 @@
     </row>
     <row r="21" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="97" t="s">
+      <c r="B22" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C22" s="97"/>
-      <c r="D22" s="97"/>
-      <c r="E22" s="97"/>
-      <c r="F22" s="97"/>
-      <c r="G22" s="97"/>
-      <c r="H22" s="97"/>
+      <c r="C22" s="110"/>
+      <c r="D22" s="110"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="110"/>
+      <c r="G22" s="110"/>
+      <c r="H22" s="110"/>
     </row>
     <row r="23" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="16" t="s">
@@ -1984,15 +1984,15 @@
     </row>
     <row r="27" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="97" t="s">
+      <c r="B28" s="110" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="97"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="97"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="97"/>
+      <c r="C28" s="110"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="110"/>
+      <c r="G28" s="110"/>
+      <c r="H28" s="110"/>
     </row>
     <row r="29" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B29" s="16" t="s">
@@ -2110,15 +2110,15 @@
     <row r="34" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="35" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="97" t="s">
+      <c r="B36" s="110" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="97"/>
-      <c r="D36" s="97"/>
-      <c r="E36" s="97"/>
-      <c r="F36" s="97"/>
-      <c r="G36" s="97"/>
-      <c r="H36" s="97"/>
+      <c r="C36" s="110"/>
+      <c r="D36" s="110"/>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="110"/>
     </row>
     <row r="37" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B37" s="16" t="s">
@@ -2236,15 +2236,15 @@
     <row r="42" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B44" s="104" t="s">
+      <c r="B44" s="111" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="104"/>
-      <c r="D44" s="104"/>
-      <c r="E44" s="104"/>
-      <c r="F44" s="104"/>
-      <c r="G44" s="104"/>
-      <c r="H44" s="104"/>
+      <c r="C44" s="111"/>
+      <c r="D44" s="111"/>
+      <c r="E44" s="111"/>
+      <c r="F44" s="111"/>
+      <c r="G44" s="111"/>
+      <c r="H44" s="111"/>
     </row>
     <row r="45" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="63" t="s">
@@ -2364,15 +2364,15 @@
     <row r="50" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="51" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="52" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="C52" s="99"/>
-      <c r="D52" s="99"/>
-      <c r="E52" s="99"/>
-      <c r="F52" s="99"/>
-      <c r="G52" s="99"/>
-      <c r="H52" s="100"/>
+      <c r="C52" s="108"/>
+      <c r="D52" s="108"/>
+      <c r="E52" s="108"/>
+      <c r="F52" s="108"/>
+      <c r="G52" s="108"/>
+      <c r="H52" s="109"/>
     </row>
     <row r="53" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B53" s="16" t="s">
@@ -2535,15 +2535,15 @@
     </row>
     <row r="62" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="97" t="s">
+      <c r="B63" s="110" t="s">
         <v>40</v>
       </c>
-      <c r="C63" s="97"/>
-      <c r="D63" s="97"/>
-      <c r="E63" s="97"/>
-      <c r="F63" s="97"/>
-      <c r="G63" s="97"/>
-      <c r="H63" s="97"/>
+      <c r="C63" s="110"/>
+      <c r="D63" s="110"/>
+      <c r="E63" s="110"/>
+      <c r="F63" s="110"/>
+      <c r="G63" s="110"/>
+      <c r="H63" s="110"/>
     </row>
     <row r="64" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
@@ -2729,15 +2729,15 @@
     <row r="73" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="75" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B75" s="98" t="s">
+      <c r="B75" s="107" t="s">
         <v>14</v>
       </c>
-      <c r="C75" s="99"/>
-      <c r="D75" s="99"/>
-      <c r="E75" s="99"/>
-      <c r="F75" s="99"/>
-      <c r="G75" s="99"/>
-      <c r="H75" s="100"/>
+      <c r="C75" s="108"/>
+      <c r="D75" s="108"/>
+      <c r="E75" s="108"/>
+      <c r="F75" s="108"/>
+      <c r="G75" s="108"/>
+      <c r="H75" s="109"/>
     </row>
     <row r="76" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B76" s="16" t="s">
@@ -2933,25 +2933,25 @@
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B87" s="108" t="s">
+      <c r="B87" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="C87" s="109" t="s">
+      <c r="C87" s="98" t="s">
         <v>20</v>
       </c>
-      <c r="D87" s="110">
+      <c r="D87" s="99">
         <v>2</v>
       </c>
-      <c r="E87" s="110" t="s">
+      <c r="E87" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="F87" s="110" t="s">
-        <v>18</v>
-      </c>
-      <c r="G87" s="110" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="111" t="s">
+      <c r="F87" s="99" t="s">
+        <v>18</v>
+      </c>
+      <c r="G87" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="100" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2980,15 +2980,15 @@
     </row>
     <row r="89" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="90" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="105" t="s">
+      <c r="B90" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="C90" s="106"/>
-      <c r="D90" s="106"/>
-      <c r="E90" s="106"/>
-      <c r="F90" s="106"/>
-      <c r="G90" s="106"/>
-      <c r="H90" s="107"/>
+      <c r="C90" s="105"/>
+      <c r="D90" s="105"/>
+      <c r="E90" s="105"/>
+      <c r="F90" s="105"/>
+      <c r="G90" s="105"/>
+      <c r="H90" s="106"/>
     </row>
     <row r="91" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B91" s="84" t="s">
@@ -3083,13 +3083,128 @@
       </c>
     </row>
     <row r="95" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B97" s="107" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="108"/>
+      <c r="D97" s="108"/>
+      <c r="E97" s="108"/>
+      <c r="F97" s="108"/>
+      <c r="G97" s="108"/>
+      <c r="H97" s="109"/>
+    </row>
+    <row r="98" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C98" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F98" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H98" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D99" s="37">
+        <v>50</v>
+      </c>
+      <c r="E99" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F99" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G99" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H99" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="100" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="101" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:8" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B102" s="107" t="s">
+        <v>12</v>
+      </c>
+      <c r="C102" s="108"/>
+      <c r="D102" s="108"/>
+      <c r="E102" s="108"/>
+      <c r="F102" s="108"/>
+      <c r="G102" s="108"/>
+      <c r="H102" s="109"/>
+    </row>
+    <row r="103" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="D103" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F103" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G103" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H103" s="16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="2:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C104" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D104" s="37">
+        <v>50</v>
+      </c>
+      <c r="E104" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="F104" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="G104" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H104" s="38" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="105" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B68:H68"/>
-    <mergeCell ref="B90:H90"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B79:H79"/>
-    <mergeCell ref="B75:H75"/>
+  <mergeCells count="15">
+    <mergeCell ref="B97:H97"/>
+    <mergeCell ref="B102:H102"/>
     <mergeCell ref="B63:H63"/>
     <mergeCell ref="B6:H6"/>
     <mergeCell ref="B22:H22"/>
@@ -3098,6 +3213,11 @@
     <mergeCell ref="B56:H56"/>
     <mergeCell ref="B36:H36"/>
     <mergeCell ref="B44:H44"/>
+    <mergeCell ref="B68:H68"/>
+    <mergeCell ref="B90:H90"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B79:H79"/>
+    <mergeCell ref="B75:H75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>